<commit_message>
Refactor code to fix position calculation for cashier 1 and limit the number of assigned cashiers to 4 per box
</commit_message>
<xml_diff>
--- a/plantilla.xlsx
+++ b/plantilla.xlsx
@@ -64,7 +64,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -104,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,17 +115,20 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,23 +432,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="43.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="43.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="43.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="43.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="8.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +460,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -469,7 +472,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -495,7 +498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -510,580 +513,576 @@
       <c r="H4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="1">
-        <v>2</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1"/>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="1">
-        <v>3</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1"/>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1">
-        <v>4</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="1">
-        <v>4</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1"/>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1">
-        <v>5</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="1">
-        <v>5</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1"/>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="1">
+        <v>5</v>
+      </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1">
-        <v>6</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="1">
-        <v>6</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="1"/>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>6</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="1">
-        <v>7</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="1">
-        <v>7</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="1"/>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="1">
+        <v>7</v>
+      </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>7</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="1">
-        <v>8</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="1">
-        <v>8</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="1"/>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="1">
+        <v>8</v>
+      </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>8</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="1">
-        <v>9</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="1">
-        <v>9</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="1"/>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="1">
+        <v>9</v>
+      </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1">
+        <v>9</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="1">
-        <v>10</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="1">
-        <v>10</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="1"/>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="1">
+        <v>10</v>
+      </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>10</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="1">
-        <v>11</v>
-      </c>
+      <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="1">
-        <v>11</v>
-      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1">
+        <v>11</v>
+      </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1">
+        <v>11</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="1">
-        <v>12</v>
-      </c>
+      <c r="A26" s="1"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="1">
-        <v>12</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1">
+        <v>12</v>
+      </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>12</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="1">
-        <v>13</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="1">
-        <v>13</v>
-      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1">
+        <v>13</v>
+      </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1">
+        <v>13</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="1">
-        <v>14</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="1">
-        <v>14</v>
-      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1">
+        <v>14</v>
+      </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="1"/>
+      <c r="E31" s="1">
+        <v>14</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="1">
-        <v>15</v>
-      </c>
+      <c r="A32" s="1"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="1">
-        <v>15</v>
-      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1">
+        <v>15</v>
+      </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1">
+        <v>15</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="1">
-        <v>16</v>
-      </c>
+      <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="1">
-        <v>16</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1">
+        <v>16</v>
+      </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1">
+        <v>16</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="1">
-        <v>17</v>
-      </c>
+      <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="1">
-        <v>17</v>
-      </c>
+      <c r="E36" s="1"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1">
+        <v>17</v>
+      </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1">
+        <v>17</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="1">
-        <v>18</v>
-      </c>
+      <c r="A38" s="1"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="1">
-        <v>18</v>
-      </c>
+      <c r="E38" s="1"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="1"/>
+      <c r="A39" s="1">
+        <v>18</v>
+      </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="4"/>
+      <c r="E39" s="1">
+        <v>18</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="1"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="1">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="A42" s="1">
         <v>20</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="1">
-        <v>20</v>
-      </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="1"/>
+      <c r="E42" s="1">
+        <v>20</v>
+      </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="1">
-        <v>21</v>
-      </c>
+      <c r="A43" s="1"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="1">
-        <v>21</v>
-      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1">
+        <v>21</v>
+      </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1">
+        <v>21</v>
+      </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="1">
-        <v>22</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="1">
-        <v>22</v>
-      </c>
+      <c r="E45" s="1"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1">
+        <v>22</v>
+      </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="1"/>
+      <c r="E46" s="1">
+        <v>22</v>
+      </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="1">
-        <v>23</v>
-      </c>
+      <c r="A47" s="1"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="1">
-        <v>23</v>
-      </c>
+      <c r="E47" s="1"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="1"/>
+      <c r="A48" s="1">
+        <v>23</v>
+      </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1">
+        <v>23</v>
+      </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="1">
-        <v>24</v>
-      </c>
+      <c r="A49" s="1"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="1">
-        <v>24</v>
-      </c>
+      <c r="E49" s="1"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1">
+        <v>24</v>
+      </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="4"/>
+      <c r="E50" s="1">
+        <v>24</v>
+      </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="1" t="s">
@@ -1095,9 +1094,9 @@
       <c r="E53" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="1" t="s">
@@ -1109,16 +1108,30 @@
       <c r="E54" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="A55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A52:H52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>